<commit_message>
first running version with Al
</commit_message>
<xml_diff>
--- a/data/WCdata_RFO.xlsx
+++ b/data/WCdata_RFO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/r_f_ott_uva_nl/Documents/Richard/PhD_ETH/matlab/14C_10Be_landscape_transience-master/My_10Be14C_codes/MCMC_inversion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/r_f_ott_uva_nl/Documents/Richard/PhD_ETH/matlab/14C_10Be_landscape_transience-master/My_10Be14C_codes/MCMC_inversion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{83DF1B2F-B15C-49C9-9C7A-A559AC6D8709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41DF73F3-3303-451B-8388-9C6566334630}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{83DF1B2F-B15C-49C9-9C7A-A559AC6D8709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8A68051-258B-41BA-9C9E-63017F100F62}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Lat</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>N14sigma</t>
+  </si>
+  <si>
+    <t>N26</t>
+  </si>
+  <si>
+    <t>N26sigma</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +483,7 @@
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -508,8 +514,14 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -540,8 +552,14 @@
       <c r="J2" s="1">
         <v>3962.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>30000</v>
+      </c>
+      <c r="L2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -573,7 +591,7 @@
         <v>3864.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -605,7 +623,7 @@
         <v>2131.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -637,7 +655,7 @@
         <v>3243</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -669,7 +687,7 @@
         <v>973.82259999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -701,7 +719,7 @@
         <v>1311.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -733,7 +751,7 @@
         <v>3977</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -765,7 +783,7 @@
         <v>3050.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -797,7 +815,7 @@
         <v>3695.8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
added functions and script to calculate isolines for single samples in spike and step model
</commit_message>
<xml_diff>
--- a/data/WCdata_RFO.xlsx
+++ b/data/WCdata_RFO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/r_f_ott_uva_nl/Documents/Richard/PhD_ETH/matlab/14C_10Be_landscape_transience-master/My_10Be14C_codes/MCMC_inversion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{83DF1B2F-B15C-49C9-9C7A-A559AC6D8709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8A68051-258B-41BA-9C9E-63017F100F62}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{83DF1B2F-B15C-49C9-9C7A-A559AC6D8709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42AB5AD1-E939-4B1C-9A39-D720CD928F29}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,12 +552,6 @@
       <c r="J2" s="1">
         <v>3962.8</v>
       </c>
-      <c r="K2">
-        <v>30000</v>
-      </c>
-      <c r="L2">
-        <v>200</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">

</xml_diff>